<commit_message>
Changes to Documentation for Usability Testing
</commit_message>
<xml_diff>
--- a/documentation/List of Jobs for Testing.xlsx
+++ b/documentation/List of Jobs for Testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\ese2018-team3\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997B8D06-A1B3-4B27-A340-2C4F3EB42ADC}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1710F118-C229-442F-84BB-574C61F413CE}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="11520" xr2:uid="{20EC7DFB-73BB-46B9-923E-5DE04EC36923}"/>
   </bookViews>
@@ -241,14 +241,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -565,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56EE912E-7BAF-44A6-835D-DFFB2B583ADC}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -585,28 +586,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E2" t="s">
@@ -652,7 +653,7 @@
       <c r="B4" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D4" t="s">
@@ -680,7 +681,7 @@
       <c r="B6" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D6" t="s">

</xml_diff>